<commit_message>
SP to BI mapped and done
</commit_message>
<xml_diff>
--- a/Master Thesis/Analys/Experiments.xlsx
+++ b/Master Thesis/Analys/Experiments.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="1" r:id="rId1"/>
     <sheet name="Times of SP" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="TimeStamps" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Measure time of total SP</t>
   </si>
@@ -189,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -278,6 +278,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -285,12 +296,6 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -298,14 +303,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,100 +410,104 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Times of SP'!$A$2:$A$33</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Times of SP'!$A$2:$A$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Times of SP'!$A$3:$A$33</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>Stored Procedure</c:v>
+                  <c:v>Report 2_6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Report 2_6</c:v>
+                  <c:v>Report 2_5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Report 2_5</c:v>
+                  <c:v>Report 3_1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Report 3_1</c:v>
+                  <c:v>Report 4_2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Report 4_2</c:v>
+                  <c:v>Report 4_4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Report 4_4</c:v>
+                  <c:v>Report 1_1_2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Report 1_1_2</c:v>
+                  <c:v>Report 1_1_1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Report 1_1_1</c:v>
+                  <c:v>Report 1_3_2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Report 1_3_2</c:v>
+                  <c:v>Report 4_3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Report 4_3</c:v>
+                  <c:v>Report 1_1_3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Report 1_1_3</c:v>
+                  <c:v>Report 1_1_9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Report 1_1_9</c:v>
+                  <c:v>Report 1_1_6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Report 1_1_6</c:v>
+                  <c:v>Report 1_1_7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Report 1_1_7</c:v>
+                  <c:v>Report 1_1_4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Report 1_1_4</c:v>
+                  <c:v>Report 1_1_5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Report 1_1_5</c:v>
+                  <c:v>Report 1_1_8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Report 1_1_8</c:v>
+                  <c:v>Report 1_2_2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Report 1_2_2</c:v>
+                  <c:v>Report 2_1_2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Report 2_1_2</c:v>
+                  <c:v>Report 1_5_7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Report 1_5_7</c:v>
+                  <c:v>Report 2_1_1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Report 2_1_1</c:v>
+                  <c:v>Report 4_5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Report 4_5</c:v>
+                  <c:v>Report 1_5_2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Report 1_5_2</c:v>
+                  <c:v>Report 1_6_1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Report 1_6_1</c:v>
+                  <c:v>Report 1_5_1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Report 1_5_1</c:v>
+                  <c:v>Report 3_7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Report 3_7</c:v>
+                  <c:v>Report 3_3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Report 3_3</c:v>
+                  <c:v>Report 3_5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Report 3_5</c:v>
+                  <c:v>Report 3_2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Report 3_2</c:v>
+                  <c:v>Report 3_4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Report 3_4</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Report 3_6</c:v>
                 </c:pt>
               </c:strCache>
@@ -500,101 +515,105 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Times of SP'!$D$2:$D$33</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Times of SP'!$D$2:$D$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Times of SP'!$D$3:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>427017</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>427017</c:v>
+                  <c:v>202116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>202116</c:v>
+                  <c:v>147443</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>147443</c:v>
+                  <c:v>33168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33168</c:v>
+                  <c:v>39300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39300</c:v>
+                  <c:v>21785</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21785</c:v>
+                  <c:v>10634</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10634</c:v>
+                  <c:v>9522</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9522</c:v>
+                  <c:v>2536</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2536</c:v>
+                  <c:v>12655</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12655</c:v>
+                  <c:v>8998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8998</c:v>
+                  <c:v>11381</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11381</c:v>
+                  <c:v>6429</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6429</c:v>
+                  <c:v>6347</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6347</c:v>
+                  <c:v>6249</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6249</c:v>
+                  <c:v>5973</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5973</c:v>
+                  <c:v>1244</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1244</c:v>
+                  <c:v>3433</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3433</c:v>
+                  <c:v>5483</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5483</c:v>
+                  <c:v>2650</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2650</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3960</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>27</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>72</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>184</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
@@ -611,11 +630,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-784221136"/>
-        <c:axId val="-784220048"/>
+        <c:axId val="-1284867344"/>
+        <c:axId val="-1284862992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-784221136"/>
+        <c:axId val="-1284867344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +677,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-784220048"/>
+        <c:crossAx val="-1284862992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -666,7 +685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-784220048"/>
+        <c:axId val="-1284862992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +736,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-784221136"/>
+        <c:crossAx val="-1284867344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -729,6 +748,669 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeStamps!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SELECT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimeStamps!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Report 2_6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Report 2_5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Report 3_1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Report 4_2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Report 4_4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report 1_1_2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Report 1_1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeStamps!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>24200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35043</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeStamps!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UPDATE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimeStamps!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Report 2_6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Report 2_5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Report 3_1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Report 4_2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Report 4_4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report 1_1_2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Report 1_1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeStamps!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>87160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeStamps!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UPDATE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimeStamps!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Report 2_6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Report 2_5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Report 3_1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Report 4_2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Report 4_4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report 1_1_2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Report 1_1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeStamps!$D$3:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7870</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeStamps!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UPDATE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimeStamps!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Report 2_6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Report 2_5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Report 3_1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Report 4_2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Report 4_4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report 1_1_2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Report 1_1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeStamps!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10850</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeStamps!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UPDATE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimeStamps!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Report 2_6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Report 2_5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Report 3_1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Report 4_2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Report 4_4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report 1_1_2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Report 1_1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeStamps!$F$3:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9573</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>473</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeStamps!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DELETE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimeStamps!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Report 2_6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Report 2_5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Report 3_1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Report 4_2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Report 4_4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report 1_1_2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Report 1_1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeStamps!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>490</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-976932496"/>
+        <c:axId val="-976943376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-976932496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-976943376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-976943376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-976932496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -806,6 +1488,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1309,20 +2031,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1633,7 +2893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1725,28 +2985,28 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickTop="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B3">
@@ -1756,12 +3016,12 @@
         <f t="shared" ref="C3:C32" si="0">SUM(B3/4)</f>
         <v>116093</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>427017</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B4">
@@ -1771,12 +3031,12 @@
         <f t="shared" si="0"/>
         <v>43648.5</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>202116</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B5">
@@ -1786,12 +3046,12 @@
         <f t="shared" si="0"/>
         <v>34500</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>147443</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B6">
@@ -1801,12 +3061,12 @@
         <f t="shared" si="0"/>
         <v>8796.75</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>33168</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
@@ -1816,12 +3076,12 @@
         <f t="shared" si="0"/>
         <v>7296.75</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>39300</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B8">
@@ -1831,12 +3091,12 @@
         <f t="shared" si="0"/>
         <v>4593.75</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>21785</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B9">
@@ -1846,12 +3106,12 @@
         <f t="shared" si="0"/>
         <v>2250.5</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>10634</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B10">
@@ -1861,12 +3121,12 @@
         <f t="shared" si="0"/>
         <v>2085.75</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>9522</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B11">
@@ -1876,12 +3136,12 @@
         <f t="shared" si="0"/>
         <v>2011.5</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>2536</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B12">
@@ -1891,12 +3151,12 @@
         <f t="shared" si="0"/>
         <v>1965</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>12655</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B13">
@@ -1906,12 +3166,12 @@
         <f t="shared" si="0"/>
         <v>1921.75</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>8998</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B14">
@@ -1921,12 +3181,12 @@
         <f t="shared" si="0"/>
         <v>1703.25</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>11381</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B15">
@@ -1936,12 +3196,12 @@
         <f t="shared" si="0"/>
         <v>1492</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>6429</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B16">
@@ -1951,12 +3211,12 @@
         <f t="shared" si="0"/>
         <v>1484.25</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <v>6347</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B17">
@@ -1966,12 +3226,12 @@
         <f t="shared" si="0"/>
         <v>1465</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>6249</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B18">
@@ -1981,12 +3241,12 @@
         <f t="shared" si="0"/>
         <v>1336</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>5973</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B19">
@@ -1996,12 +3256,12 @@
         <f t="shared" si="0"/>
         <v>1113</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>1244</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B20">
@@ -2011,12 +3271,12 @@
         <f t="shared" si="0"/>
         <v>781.25</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <v>3433</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B21">
@@ -2026,12 +3286,12 @@
         <f t="shared" si="0"/>
         <v>773.5</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>5483</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B22">
@@ -2041,12 +3301,12 @@
         <f t="shared" si="0"/>
         <v>590</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="5">
         <v>2650</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B23">
@@ -2056,12 +3316,12 @@
         <f t="shared" si="0"/>
         <v>304.25</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <v>3960</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B24">
@@ -2071,12 +3331,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B25">
@@ -2086,12 +3346,12 @@
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B26">
@@ -2101,12 +3361,12 @@
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B27">
@@ -2116,12 +3376,12 @@
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B28">
@@ -2131,12 +3391,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B29">
@@ -2146,12 +3406,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B30">
@@ -2161,12 +3421,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="5">
         <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B31">
@@ -2176,12 +3436,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B32">
@@ -2191,7 +3451,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="5">
         <v>34</v>
       </c>
     </row>
@@ -2207,10 +3467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2218,11 +3478,8 @@
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1">
-      <c r="A1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="B1" s="12" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="11"/>
@@ -2230,10 +3487,11 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" thickBot="1">
-      <c r="A2" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickTop="1">
+      <c r="A2" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
@@ -2250,53 +3508,86 @@
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" thickTop="1">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="8" t="s">
+      <c r="B3">
+        <v>24200</v>
+      </c>
+      <c r="C3">
+        <v>87160</v>
+      </c>
+      <c r="D3">
+        <v>10020</v>
+      </c>
+      <c r="E3">
+        <v>10850</v>
+      </c>
+      <c r="F3">
+        <v>9573</v>
+      </c>
+      <c r="G3">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="8" t="s">
+      <c r="B4">
+        <v>35043</v>
+      </c>
+      <c r="C4">
+        <v>9116</v>
+      </c>
+      <c r="D4">
+        <v>7870</v>
+      </c>
+      <c r="E4">
+        <v>10140</v>
+      </c>
+      <c r="F4">
+        <v>473</v>
+      </c>
+      <c r="G4">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
worst parts of sp identified
</commit_message>
<xml_diff>
--- a/Master Thesis/Analys/Experiments.xlsx
+++ b/Master Thesis/Analys/Experiments.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="1" r:id="rId1"/>
     <sheet name="Times of SP" sheetId="2" r:id="rId2"/>
     <sheet name="TimeStamps" sheetId="3" r:id="rId3"/>
+    <sheet name="Troublepart of SP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Measure time of total SP</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Report 3_6</t>
   </si>
   <si>
-    <t>SELECT</t>
-  </si>
-  <si>
     <t>UPDATE</t>
   </si>
   <si>
@@ -160,6 +158,9 @@
   </si>
   <si>
     <t>Stored Procedures</t>
+  </si>
+  <si>
+    <t>INSERT</t>
   </si>
 </sst>
 </file>
@@ -175,18 +176,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -295,29 +290,29 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,11 +625,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1284867344"/>
-        <c:axId val="-1284862992"/>
+        <c:axId val="2116993280"/>
+        <c:axId val="2116982400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1284867344"/>
+        <c:axId val="2116993280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,7 +672,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1284862992"/>
+        <c:crossAx val="2116982400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -685,7 +680,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1284862992"/>
+        <c:axId val="2116982400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +731,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1284867344"/>
+        <c:crossAx val="2116993280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -846,7 +841,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SELECT</c:v>
+                  <c:v>INSERT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -902,6 +897,21 @@
                 <c:pt idx="1">
                   <c:v>35043</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>4806</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8134</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12264</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12010</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10710</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -971,6 +981,15 @@
                 <c:pt idx="1">
                   <c:v>9116</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>45713</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1040,6 +1059,15 @@
                 <c:pt idx="1">
                   <c:v>7870</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>24616</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1109,6 +1137,15 @@
                 <c:pt idx="1">
                   <c:v>10140</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1247,6 +1284,9 @@
                 <c:pt idx="1">
                   <c:v>490</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1261,11 +1301,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-976932496"/>
-        <c:axId val="-976943376"/>
+        <c:axId val="2116771760"/>
+        <c:axId val="2116776112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-976932496"/>
+        <c:axId val="2116771760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1348,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-976943376"/>
+        <c:crossAx val="2116776112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1316,7 +1356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-976943376"/>
+        <c:axId val="2116776112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,7 +1407,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-976932496"/>
+        <c:crossAx val="2116771760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2539,15 +2579,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2573,16 +2613,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2893,7 +2933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2973,485 +3013,486 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="B11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickTop="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>464372</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <f t="shared" ref="C3:C32" si="0">SUM(B3/4)</f>
         <v>116093</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="12">
         <v>427017</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>174594</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>43648.5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="12">
         <v>202116</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>138000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>34500</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="12">
         <v>147443</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>35187</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>8796.75</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="12">
         <v>33168</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>29187</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>7296.75</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="12">
         <v>39300</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>18375</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4593.75</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="12">
         <v>21785</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>9002</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>2250.5</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="12">
         <v>10634</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>8343</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>2085.75</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="12">
         <v>9522</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>8046</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>2011.5</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="12">
         <v>2536</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>7860</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>1965</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="12">
         <v>12655</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>7687</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>1921.75</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="12">
         <v>8998</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>6813</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>1703.25</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="12">
         <v>11381</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>5968</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>1492</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="12">
         <v>6429</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>5937</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>1484.25</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="12">
         <v>6347</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>5860</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>1465</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="12">
         <v>6249</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>5344</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>1336</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="12">
         <v>5973</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>4452</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>1113</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="12">
         <v>1244</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>3125</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>781.25</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="12">
         <v>3433</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>3094</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>773.5</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="12">
         <v>5483</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>2360</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>590</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="12">
         <v>2650</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>1217</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>304.25</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="12">
         <v>3960</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>32</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="12">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>31</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="12">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>31</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="12">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>31</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="12">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>16</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="12">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>16</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="12">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>16</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="12">
         <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="12">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="12">
         <v>34</v>
       </c>
     </row>
@@ -3469,117 +3510,163 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickTop="1">
+      <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>24200</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>87160</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>10020</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>10850</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>9573</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>565</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>35043</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>9116</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>7870</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>10140</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>473</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B5" s="2">
+        <v>4806</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45713</v>
+      </c>
+      <c r="D5" s="2">
+        <v>24616</v>
+      </c>
+      <c r="E5" s="2">
+        <v>243</v>
+      </c>
+      <c r="G5" s="2">
+        <v>514</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="B6" s="2">
+        <v>8134</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B7" s="2">
+        <v>12264</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B8" s="2">
+        <v>12010</v>
+      </c>
+      <c r="C8" s="2">
+        <v>223</v>
+      </c>
+      <c r="D8" s="2">
+        <v>246</v>
+      </c>
+      <c r="E8" s="2">
+        <v>328</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10710</v>
+      </c>
+      <c r="C9" s="2">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2">
+        <v>70</v>
+      </c>
+      <c r="E9" s="12">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3590,4 +3677,91 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="16.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>INDEX(TimeStamps!$B$2:$G$2,,MATCH(MAX(TimeStamps!B3:G3),TimeStamps!B3:G3,0))</f>
+        <v>UPDATE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>INDEX(TimeStamps!$B$2:$G$2,,MATCH(MAX(TimeStamps!B4:G4),TimeStamps!B4:G4,0))</f>
+        <v>INSERT</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>INDEX(TimeStamps!$B$2:$G$2,,MATCH(MAX(TimeStamps!B5:G5),TimeStamps!B5:G5,0))</f>
+        <v>UPDATE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>INDEX(TimeStamps!$B$2:$G$2,,MATCH(MAX(TimeStamps!B6:G6),TimeStamps!B6:G6,0))</f>
+        <v>INSERT</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>INDEX(TimeStamps!$B$2:$G$2,,MATCH(MAX(TimeStamps!B7:G7),TimeStamps!B7:G7,0))</f>
+        <v>INSERT</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>INDEX(TimeStamps!$B$2:$G$2,,MATCH(MAX(TimeStamps!B8:G8),TimeStamps!B8:G8,0))</f>
+        <v>INSERT</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>INDEX(TimeStamps!$B$2:$G$2,,MATCH(MAX(TimeStamps!B9:G9),TimeStamps!B9:G9,0))</f>
+        <v>INSERT</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2_6 done with index and keys
</commit_message>
<xml_diff>
--- a/Master Thesis/Analys/Experiments.xlsx
+++ b/Master Thesis/Analys/Experiments.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Table content drop w I&amp;Keys" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -205,7 +204,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -342,11 +341,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -367,6 +390,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -699,11 +725,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="723981376"/>
-        <c:axId val="723982464"/>
+        <c:axId val="-1524066528"/>
+        <c:axId val="-1524071424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="723981376"/>
+        <c:axId val="-1524066528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +772,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723982464"/>
+        <c:crossAx val="-1524071424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -754,7 +780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="723982464"/>
+        <c:axId val="-1524071424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,9 +831,274 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723981376"/>
+        <c:crossAx val="-1524066528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Table content drop w I&amp;Keys'!$A$3:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10447188</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9706149</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6945334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3726035</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>280859</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Table content drop w I&amp;Keys'!$B$3:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>145645</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>177675</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>127056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31979</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1310571216"/>
+        <c:axId val="-1310568496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1310571216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1310568496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1310568496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1310571216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1374,11 +1665,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="723974304"/>
-        <c:axId val="723969952"/>
+        <c:axId val="-1311397728"/>
+        <c:axId val="-1311394464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="723974304"/>
+        <c:axId val="-1311397728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,7 +1712,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723969952"/>
+        <c:crossAx val="-1311394464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1429,7 +1720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="723969952"/>
+        <c:axId val="-1311394464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1480,7 +1771,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723974304"/>
+        <c:crossAx val="-1311397728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1597,23 +1888,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$A$3:$A$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>10447188</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9706149</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6945334</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3726035</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>280859</c:v>
                 </c:pt>
               </c:numCache>
@@ -1621,23 +1912,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$B$3:$B$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>253501</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>236662</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>171116</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>102429</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>34252</c:v>
                 </c:pt>
               </c:numCache>
@@ -1653,11 +1944,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="723967776"/>
-        <c:axId val="723977568"/>
+        <c:axId val="-1311405344"/>
+        <c:axId val="-1311406432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="723967776"/>
+        <c:axId val="-1311405344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,12 +2005,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723977568"/>
+        <c:crossAx val="-1311406432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="723977568"/>
+        <c:axId val="-1311406432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,7 +2067,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723967776"/>
+        <c:crossAx val="-1311405344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1862,23 +2153,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$G$3:$G$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$G$3:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>10447188</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9706149</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6945334</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3726035</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>280859</c:v>
                 </c:pt>
               </c:numCache>
@@ -1886,23 +2177,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$H$3:$H$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$H$3:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>1328</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1372</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>4671</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4854</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -1918,11 +2209,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="723819424"/>
-        <c:axId val="881607568"/>
+        <c:axId val="-1311405888"/>
+        <c:axId val="-1311397184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="723819424"/>
+        <c:axId val="-1311405888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,12 +2270,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881607568"/>
+        <c:crossAx val="-1311397184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="881607568"/>
+        <c:axId val="-1311397184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2041,7 +2332,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="723819424"/>
+        <c:crossAx val="-1311405888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2127,23 +2418,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$I$3:$I$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$I$3:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>10447188</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9706149</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6945334</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3726035</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>280859</c:v>
                 </c:pt>
               </c:numCache>
@@ -2151,23 +2442,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$J$3:$J$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$J$3:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>2129</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1947</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1370</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1079</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
@@ -2183,11 +2474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="881616816"/>
-        <c:axId val="881602672"/>
+        <c:axId val="-1311393920"/>
+        <c:axId val="-1311395552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="881616816"/>
+        <c:axId val="-1311393920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2244,12 +2535,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881602672"/>
+        <c:crossAx val="-1311395552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="881602672"/>
+        <c:axId val="-1311395552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2306,7 +2597,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881616816"/>
+        <c:crossAx val="-1311393920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2392,23 +2683,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$C$3:$C$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>39869</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>29876</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>19883</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>11053</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>724</c:v>
                 </c:pt>
               </c:numCache>
@@ -2416,23 +2707,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$D$3:$D$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$D$3:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>64036</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>50437</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>37977</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>22819</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>124</c:v>
                 </c:pt>
               </c:numCache>
@@ -2448,11 +2739,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="881612464"/>
-        <c:axId val="881607024"/>
+        <c:axId val="-1311408064"/>
+        <c:axId val="-1311404800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="881612464"/>
+        <c:axId val="-1311408064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2509,12 +2800,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881607024"/>
+        <c:crossAx val="-1311404800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="881607024"/>
+        <c:axId val="-1311404800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,7 +2862,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881612464"/>
+        <c:crossAx val="-1311408064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2657,23 +2948,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$E$3:$E$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$E$3:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>2732242</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2572413</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1821520</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>978797</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>71366</c:v>
                 </c:pt>
               </c:numCache>
@@ -2681,23 +2972,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$F$3:$F$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$F$3:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
                   <c:v>83848</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>67341</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>52987</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>40827</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>31625</c:v>
                 </c:pt>
               </c:numCache>
@@ -2713,11 +3004,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="881611376"/>
-        <c:axId val="881604848"/>
+        <c:axId val="-1311403712"/>
+        <c:axId val="-1311407520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="881611376"/>
+        <c:axId val="-1311403712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2774,12 +3065,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881604848"/>
+        <c:crossAx val="-1311407520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="881604848"/>
+        <c:axId val="-1311407520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,7 +3127,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881611376"/>
+        <c:crossAx val="-1311403712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2922,23 +3213,26 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$K$3:$K$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$K$3:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>79738</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>39869</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>29876</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>19883</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>11053</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>724</c:v>
                 </c:pt>
               </c:numCache>
@@ -2946,23 +3240,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$L$3:$L$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$L$3:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>23580</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>11983</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>11126</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>10769</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6137</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -2978,11 +3275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="881608656"/>
-        <c:axId val="881611920"/>
+        <c:axId val="-1311402080"/>
+        <c:axId val="-1311401536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="881608656"/>
+        <c:axId val="-1311402080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3039,12 +3336,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881611920"/>
+        <c:crossAx val="-1311401536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="881611920"/>
+        <c:axId val="-1311401536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3101,7 +3398,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881608656"/>
+        <c:crossAx val="-1311402080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3187,23 +3484,26 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$M$3:$M$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$M$3:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>79738</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>39869</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>29876</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>19883</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>11053</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>724</c:v>
                 </c:pt>
               </c:numCache>
@@ -3211,23 +3511,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table content drop wo I&amp;Keys'!$N$3:$N$15</c:f>
+              <c:f>'Table content drop wo I&amp;Keys'!$N$3:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>20500</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10343</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9671</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8947</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5278</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -3243,11 +3546,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="881609200"/>
-        <c:axId val="881605392"/>
+        <c:axId val="-1311398272"/>
+        <c:axId val="-1310569040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="881609200"/>
+        <c:axId val="-1311398272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,12 +3607,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881605392"/>
+        <c:crossAx val="-1310569040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="881605392"/>
+        <c:axId val="-1310569040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3366,7 +3669,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881609200"/>
+        <c:crossAx val="-1311398272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3416,6 +3719,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4278,6 +4621,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -8469,13 +9328,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8499,13 +9358,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8529,13 +9388,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1562100</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8559,13 +9418,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1543050</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8589,13 +9448,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1557337</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1571625</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8617,16 +9476,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1571625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>6804</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>10205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>23133</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>172811</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8649,13 +9508,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8670,6 +9529,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9060,11 +9954,11 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
@@ -9555,14 +10449,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1">
       <c r="A2" s="1" t="s">
@@ -9832,10 +10726,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q9" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9845,41 +10739,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1">
-      <c r="A1" s="24" t="str">
+      <c r="A1" s="27" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A2," - ",'Troublepart of SP'!$C2)</f>
         <v>Report 2_6 - EXT_HISTORY_MASTER</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23" t="str">
+      <c r="B1" s="25"/>
+      <c r="C1" s="26" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A3," - ",'Troublepart of SP'!$C3)</f>
         <v>Report 2_5 - EXT_ITEM</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="22" t="str">
+      <c r="D1" s="27"/>
+      <c r="E1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A4," - ",'Troublepart of SP'!$C4)</f>
         <v>Report 3_1 - EXT_ITEM_LEDGER_ENTRY</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="str">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A5," - ",'Troublepart of SP'!$C5)</f>
         <v>Report 4_2 - EXT_HISTORY_MASTER</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22" t="str">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A6," - ",'Troublepart of SP'!$C6)</f>
         <v>Report 4_4 - EXT_HISTORY_MASTER</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22" t="str">
+      <c r="J1" s="25"/>
+      <c r="K1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A7," - ",'Troublepart of SP'!$C7)</f>
         <v>Report 1_1_2 - EXT_ITEM</v>
       </c>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22" t="str">
+      <c r="L1" s="25"/>
+      <c r="M1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A8," - ",'Troublepart of SP'!$C8)</f>
         <v>Report 1_1_1 - EXT_ITEM</v>
       </c>
-      <c r="N1" s="23"/>
+      <c r="N1" s="26"/>
     </row>
     <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1">
       <c r="A2" s="11" t="s">
@@ -9925,233 +10819,249 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:14" customFormat="1">
-      <c r="A3">
-        <v>10447188</v>
-      </c>
-      <c r="B3" s="14">
-        <v>253501</v>
-      </c>
-      <c r="C3" s="10">
-        <v>39869</v>
-      </c>
-      <c r="D3" s="14">
-        <v>64036</v>
-      </c>
-      <c r="E3" s="17">
-        <v>2732242</v>
-      </c>
-      <c r="F3" s="15">
-        <v>83848</v>
-      </c>
-      <c r="G3">
-        <v>10447188</v>
-      </c>
-      <c r="H3" s="15">
-        <v>1328</v>
-      </c>
-      <c r="I3">
-        <v>10447188</v>
-      </c>
-      <c r="J3" s="15">
-        <v>2129</v>
-      </c>
-      <c r="K3" s="10">
-        <v>39869</v>
-      </c>
-      <c r="L3" s="15">
-        <v>11983</v>
-      </c>
-      <c r="M3" s="10">
-        <v>39869</v>
-      </c>
-      <c r="N3" s="17">
-        <v>10343</v>
+    <row r="3" spans="1:14" customFormat="1" ht="15" thickBot="1">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="18">
+        <v>79738</v>
+      </c>
+      <c r="L3" s="19">
+        <v>23580</v>
+      </c>
+      <c r="M3" s="18">
+        <v>79738</v>
+      </c>
+      <c r="N3" s="20">
+        <v>20500</v>
       </c>
     </row>
     <row r="4" spans="1:14" customFormat="1">
       <c r="A4">
-        <v>9706149</v>
+        <v>10447188</v>
       </c>
       <c r="B4" s="14">
-        <v>236662</v>
+        <v>253501</v>
       </c>
       <c r="C4" s="10">
-        <v>29876</v>
+        <v>39869</v>
       </c>
       <c r="D4" s="14">
-        <v>50437</v>
-      </c>
-      <c r="E4" s="10">
-        <v>2572413</v>
+        <v>64036</v>
+      </c>
+      <c r="E4" s="17">
+        <v>2732242</v>
       </c>
       <c r="F4" s="15">
-        <v>67341</v>
+        <v>83848</v>
       </c>
       <c r="G4">
-        <v>9706149</v>
+        <v>10447188</v>
       </c>
       <c r="H4" s="15">
-        <v>1372</v>
+        <v>1328</v>
       </c>
       <c r="I4">
-        <v>9706149</v>
+        <v>10447188</v>
       </c>
       <c r="J4" s="15">
-        <v>1947</v>
+        <v>2129</v>
       </c>
       <c r="K4" s="10">
-        <v>29876</v>
+        <v>39869</v>
       </c>
       <c r="L4" s="15">
-        <v>11126</v>
+        <v>11983</v>
       </c>
       <c r="M4" s="10">
-        <v>29876</v>
-      </c>
-      <c r="N4">
-        <v>9671</v>
+        <v>39869</v>
+      </c>
+      <c r="N4" s="17">
+        <v>10343</v>
       </c>
     </row>
     <row r="5" spans="1:14" customFormat="1">
       <c r="A5">
-        <v>6945334</v>
+        <v>9706149</v>
       </c>
       <c r="B5" s="14">
-        <v>171116</v>
+        <v>236662</v>
       </c>
       <c r="C5" s="10">
-        <v>19883</v>
+        <v>29876</v>
       </c>
       <c r="D5" s="14">
-        <v>37977</v>
+        <v>50437</v>
       </c>
       <c r="E5" s="10">
-        <v>1821520</v>
+        <v>2572413</v>
       </c>
       <c r="F5" s="15">
-        <v>52987</v>
+        <v>67341</v>
       </c>
       <c r="G5">
-        <v>6945334</v>
+        <v>9706149</v>
       </c>
       <c r="H5" s="15">
-        <v>4671</v>
+        <v>1372</v>
       </c>
       <c r="I5">
-        <v>6945334</v>
+        <v>9706149</v>
       </c>
       <c r="J5" s="15">
-        <v>1370</v>
+        <v>1947</v>
       </c>
       <c r="K5" s="10">
-        <v>19883</v>
+        <v>29876</v>
       </c>
       <c r="L5" s="15">
-        <v>10769</v>
+        <v>11126</v>
       </c>
       <c r="M5" s="10">
-        <v>19883</v>
+        <v>29876</v>
       </c>
       <c r="N5">
-        <v>8947</v>
+        <v>9671</v>
       </c>
     </row>
     <row r="6" spans="1:14" customFormat="1">
       <c r="A6">
-        <v>3726035</v>
+        <v>6945334</v>
       </c>
       <c r="B6" s="14">
-        <v>102429</v>
+        <v>171116</v>
       </c>
       <c r="C6" s="10">
-        <v>11053</v>
+        <v>19883</v>
       </c>
       <c r="D6" s="14">
-        <v>22819</v>
+        <v>37977</v>
       </c>
       <c r="E6" s="10">
-        <v>978797</v>
+        <v>1821520</v>
       </c>
       <c r="F6" s="15">
-        <v>40827</v>
+        <v>52987</v>
       </c>
       <c r="G6">
-        <v>3726035</v>
+        <v>6945334</v>
       </c>
       <c r="H6" s="15">
-        <v>4854</v>
+        <v>4671</v>
       </c>
       <c r="I6">
-        <v>3726035</v>
+        <v>6945334</v>
       </c>
       <c r="J6" s="15">
-        <v>1079</v>
+        <v>1370</v>
       </c>
       <c r="K6" s="10">
-        <v>11053</v>
+        <v>19883</v>
       </c>
       <c r="L6" s="15">
-        <v>6137</v>
+        <v>10769</v>
       </c>
       <c r="M6" s="10">
-        <v>11053</v>
+        <v>19883</v>
       </c>
       <c r="N6">
-        <v>5278</v>
+        <v>8947</v>
       </c>
     </row>
     <row r="7" spans="1:14" customFormat="1">
       <c r="A7">
-        <v>280859</v>
+        <v>3726035</v>
       </c>
       <c r="B7" s="14">
-        <v>34252</v>
+        <v>102429</v>
       </c>
       <c r="C7" s="10">
-        <v>724</v>
+        <v>11053</v>
       </c>
       <c r="D7" s="14">
-        <v>124</v>
+        <v>22819</v>
       </c>
       <c r="E7" s="10">
-        <v>71366</v>
+        <v>978797</v>
       </c>
       <c r="F7" s="15">
-        <v>31625</v>
+        <v>40827</v>
       </c>
       <c r="G7">
-        <v>280859</v>
+        <v>3726035</v>
       </c>
       <c r="H7" s="15">
-        <v>11</v>
+        <v>4854</v>
       </c>
       <c r="I7">
-        <v>280859</v>
+        <v>3726035</v>
       </c>
       <c r="J7" s="15">
-        <v>60</v>
+        <v>1079</v>
       </c>
       <c r="K7" s="10">
-        <v>724</v>
+        <v>11053</v>
       </c>
       <c r="L7" s="15">
-        <v>15</v>
+        <v>6137</v>
       </c>
       <c r="M7" s="10">
-        <v>724</v>
+        <v>11053</v>
       </c>
       <c r="N7">
-        <v>11</v>
+        <v>5278</v>
       </c>
     </row>
     <row r="8" spans="1:14" customFormat="1">
-      <c r="B8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="A8">
+        <v>280859</v>
+      </c>
+      <c r="B8" s="14">
+        <v>34252</v>
+      </c>
+      <c r="C8" s="10">
+        <v>724</v>
+      </c>
+      <c r="D8" s="14">
+        <v>124</v>
+      </c>
+      <c r="E8" s="10">
+        <v>71366</v>
+      </c>
+      <c r="F8" s="15">
+        <v>31625</v>
+      </c>
+      <c r="G8">
+        <v>280859</v>
+      </c>
+      <c r="H8" s="15">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>280859</v>
+      </c>
+      <c r="J8" s="15">
+        <v>60</v>
+      </c>
+      <c r="K8" s="10">
+        <v>724</v>
+      </c>
+      <c r="L8" s="15">
+        <v>15</v>
+      </c>
+      <c r="M8" s="10">
+        <v>724</v>
+      </c>
+      <c r="N8">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:14" customFormat="1">
       <c r="B9" s="15"/>
@@ -10209,6 +11119,22 @@
       <c r="J15" s="15"/>
       <c r="L15" s="15"/>
     </row>
+    <row r="16" spans="1:14">
+      <c r="A16"/>
+      <c r="B16" s="15"/>
+      <c r="C16"/>
+      <c r="D16" s="15"/>
+      <c r="E16"/>
+      <c r="F16" s="15"/>
+      <c r="G16"/>
+      <c r="H16" s="15"/>
+      <c r="I16"/>
+      <c r="J16" s="15"/>
+      <c r="K16"/>
+      <c r="L16" s="15"/>
+      <c r="M16"/>
+      <c r="N16"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="K1:L1"/>
@@ -10230,7 +11156,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10240,41 +11166,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1">
-      <c r="A1" s="24" t="str">
+      <c r="A1" s="27" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A2," - ",'Troublepart of SP'!$C2)</f>
         <v>Report 2_6 - EXT_HISTORY_MASTER</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23" t="str">
+      <c r="B1" s="25"/>
+      <c r="C1" s="26" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A3," - ",'Troublepart of SP'!$C3)</f>
         <v>Report 2_5 - EXT_ITEM</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="22" t="str">
+      <c r="D1" s="27"/>
+      <c r="E1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A4," - ",'Troublepart of SP'!$C4)</f>
         <v>Report 3_1 - EXT_ITEM_LEDGER_ENTRY</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="str">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A5," - ",'Troublepart of SP'!$C5)</f>
         <v>Report 4_2 - EXT_HISTORY_MASTER</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22" t="str">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A6," - ",'Troublepart of SP'!$C6)</f>
         <v>Report 4_4 - EXT_HISTORY_MASTER</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22" t="str">
+      <c r="J1" s="25"/>
+      <c r="K1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A7," - ",'Troublepart of SP'!$C7)</f>
         <v>Report 1_1_2 - EXT_ITEM</v>
       </c>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22" t="str">
+      <c r="L1" s="25"/>
+      <c r="M1" s="25" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A8," - ",'Troublepart of SP'!$C8)</f>
         <v>Report 1_1_1 - EXT_ITEM</v>
       </c>
-      <c r="N1" s="23"/>
+      <c r="N1" s="26"/>
     </row>
     <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1">
       <c r="A2" s="11" t="s">
@@ -10324,7 +11250,9 @@
       <c r="A3">
         <v>10447188</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="15">
+        <v>145645</v>
+      </c>
       <c r="C3" s="10">
         <v>39869</v>
       </c>
@@ -10336,7 +11264,7 @@
       <c r="G3">
         <v>10447188</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="16"/>
       <c r="I3">
         <v>10447188</v>
       </c>
@@ -10354,7 +11282,9 @@
       <c r="A4">
         <v>9706149</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="14">
+        <v>177675</v>
+      </c>
       <c r="C4" s="10">
         <v>29876</v>
       </c>
@@ -10383,7 +11313,9 @@
       <c r="A5">
         <v>6945334</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="14">
+        <v>127056</v>
+      </c>
       <c r="C5" s="10">
         <v>19883</v>
       </c>
@@ -10412,7 +11344,9 @@
       <c r="A6">
         <v>3726035</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="14">
+        <v>81026</v>
+      </c>
       <c r="C6" s="10">
         <v>11053</v>
       </c>
@@ -10441,7 +11375,9 @@
       <c r="A7">
         <v>280859</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="14">
+        <v>31979</v>
+      </c>
       <c r="C7" s="10">
         <v>724</v>
       </c>
@@ -10541,5 +11477,7 @@
     <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all done with time measurment on tables wo keys and index
</commit_message>
<xml_diff>
--- a/Master Thesis/Analys/Experiments.xlsx
+++ b/Master Thesis/Analys/Experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,11 +725,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1524066528"/>
-        <c:axId val="-1524071424"/>
+        <c:axId val="-40145008"/>
+        <c:axId val="-40149904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1524066528"/>
+        <c:axId val="-40145008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +772,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1524071424"/>
+        <c:crossAx val="-40149904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -780,7 +780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1524071424"/>
+        <c:axId val="-40149904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +831,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1524066528"/>
+        <c:crossAx val="-40145008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,11 +973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1310571216"/>
-        <c:axId val="-1310568496"/>
+        <c:axId val="-2012877696"/>
+        <c:axId val="-2012874976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1310571216"/>
+        <c:axId val="-2012877696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,12 +1034,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1310568496"/>
+        <c:crossAx val="-2012874976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1310568496"/>
+        <c:axId val="-2012874976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,7 +1096,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1310571216"/>
+        <c:crossAx val="-2012877696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1665,11 +1665,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1311397728"/>
-        <c:axId val="-1311394464"/>
+        <c:axId val="-40148816"/>
+        <c:axId val="-40136848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1311397728"/>
+        <c:axId val="-40148816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,7 +1712,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311394464"/>
+        <c:crossAx val="-40136848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1720,7 +1720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1311394464"/>
+        <c:axId val="-40136848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1771,7 +1771,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311397728"/>
+        <c:crossAx val="-40148816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1892,6 +1892,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>17449200</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>10447188</c:v>
                 </c:pt>
@@ -1916,6 +1919,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>403186</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>253501</c:v>
                 </c:pt>
@@ -1944,11 +1950,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311405344"/>
-        <c:axId val="-1311406432"/>
+        <c:axId val="-40147728"/>
+        <c:axId val="-40144464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311405344"/>
+        <c:axId val="-40147728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2005,12 +2011,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311406432"/>
+        <c:crossAx val="-40144464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1311406432"/>
+        <c:axId val="-40144464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2067,7 +2073,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311405344"/>
+        <c:crossAx val="-40147728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2157,6 +2163,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>17449200</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>10447188</c:v>
                 </c:pt>
@@ -2181,6 +2190,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1427</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1328</c:v>
                 </c:pt>
@@ -2209,11 +2221,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311405888"/>
-        <c:axId val="-1311397184"/>
+        <c:axId val="-40138480"/>
+        <c:axId val="-40142288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311405888"/>
+        <c:axId val="-40138480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2270,12 +2282,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311397184"/>
+        <c:crossAx val="-40142288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1311397184"/>
+        <c:axId val="-40142288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2344,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311405888"/>
+        <c:crossAx val="-40138480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2422,6 +2434,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>17449200</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>10447188</c:v>
                 </c:pt>
@@ -2446,6 +2461,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3413</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>2129</c:v>
                 </c:pt>
@@ -2474,11 +2492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311393920"/>
-        <c:axId val="-1311395552"/>
+        <c:axId val="-40137936"/>
+        <c:axId val="-2013222448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311393920"/>
+        <c:axId val="-40137936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2535,12 +2553,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311395552"/>
+        <c:crossAx val="-2013222448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1311395552"/>
+        <c:axId val="-2013222448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2597,7 +2615,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311393920"/>
+        <c:crossAx val="-40137936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2687,6 +2705,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>69409</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>39869</c:v>
                 </c:pt>
@@ -2711,6 +2732,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>83584</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>64036</c:v>
                 </c:pt>
@@ -2739,11 +2763,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311408064"/>
-        <c:axId val="-1311404800"/>
+        <c:axId val="-2013218640"/>
+        <c:axId val="-2013218096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311408064"/>
+        <c:axId val="-2013218640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2800,12 +2824,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311404800"/>
+        <c:crossAx val="-2013218096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1311404800"/>
+        <c:axId val="-2013218096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2862,7 +2886,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311408064"/>
+        <c:crossAx val="-2013218640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2952,6 +2976,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>4557053</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>2732242</c:v>
                 </c:pt>
@@ -2976,6 +3003,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>104503</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>83848</c:v>
                 </c:pt>
@@ -3004,11 +3034,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311403712"/>
-        <c:axId val="-1311407520"/>
+        <c:axId val="-2013219728"/>
+        <c:axId val="-2013217552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311403712"/>
+        <c:axId val="-2013219728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3065,12 +3095,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311407520"/>
+        <c:crossAx val="-2013217552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1311407520"/>
+        <c:axId val="-2013217552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3127,7 +3157,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311403712"/>
+        <c:crossAx val="-2013219728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3218,7 +3248,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>79738</c:v>
+                  <c:v>69409</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>39869</c:v>
@@ -3245,7 +3275,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>23580</c:v>
+                  <c:v>18111</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11983</c:v>
@@ -3275,11 +3305,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311402080"/>
-        <c:axId val="-1311401536"/>
+        <c:axId val="-2013220272"/>
+        <c:axId val="-2013222992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311402080"/>
+        <c:axId val="-2013220272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,12 +3366,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311401536"/>
+        <c:crossAx val="-2013222992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1311401536"/>
+        <c:axId val="-2013222992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3398,7 +3428,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311402080"/>
+        <c:crossAx val="-2013220272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3489,7 +3519,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>79738</c:v>
+                  <c:v>69409</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>39869</c:v>
@@ -3516,7 +3546,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>20500</c:v>
+                  <c:v>15218</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10343</c:v>
@@ -3546,11 +3576,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311398272"/>
-        <c:axId val="-1310569040"/>
+        <c:axId val="-2012873344"/>
+        <c:axId val="-2012873888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311398272"/>
+        <c:axId val="-2012873344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3607,12 +3637,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1310569040"/>
+        <c:crossAx val="-2012873888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1310569040"/>
+        <c:axId val="-2012873888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3669,7 +3699,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311398272"/>
+        <c:crossAx val="-2012873344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9865,9 +9895,9 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -9875,7 +9905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -9883,7 +9913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -9891,7 +9921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -9899,7 +9929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -9907,7 +9937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -9915,7 +9945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -9923,7 +9953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -9944,7 +9974,7 @@
       <selection activeCell="B11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" style="2" bestFit="1" customWidth="1"/>
@@ -9952,7 +9982,7 @@
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="21" t="s">
         <v>8</v>
@@ -9960,7 +9990,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -9974,7 +10004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickTop="1">
+    <row r="3" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -9989,7 +10019,7 @@
         <v>427017</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -10004,7 +10034,7 @@
         <v>202116</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -10019,7 +10049,7 @@
         <v>147443</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -10034,7 +10064,7 @@
         <v>33168</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -10049,7 +10079,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -10064,7 +10094,7 @@
         <v>21785</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -10079,7 +10109,7 @@
         <v>10634</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -10094,7 +10124,7 @@
         <v>9522</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -10109,7 +10139,7 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -10124,7 +10154,7 @@
         <v>12655</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -10139,7 +10169,7 @@
         <v>8998</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -10154,7 +10184,7 @@
         <v>11381</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -10169,7 +10199,7 @@
         <v>6429</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -10184,7 +10214,7 @@
         <v>6347</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -10199,7 +10229,7 @@
         <v>6249</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
@@ -10214,7 +10244,7 @@
         <v>5973</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -10229,7 +10259,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -10244,7 +10274,7 @@
         <v>3433</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
@@ -10259,7 +10289,7 @@
         <v>5483</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>32</v>
       </c>
@@ -10274,7 +10304,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
@@ -10289,7 +10319,7 @@
         <v>3960</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
@@ -10304,7 +10334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -10319,7 +10349,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -10334,7 +10364,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>37</v>
       </c>
@@ -10349,7 +10379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -10364,7 +10394,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
@@ -10379,7 +10409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -10394,7 +10424,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
@@ -10409,7 +10439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>42</v>
       </c>
@@ -10424,7 +10454,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" ht="15" thickTop="1"/>
+    <row r="33" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
@@ -10442,13 +10472,13 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="23" t="s">
         <v>45</v>
       </c>
@@ -10458,7 +10488,7 @@
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1">
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -10481,7 +10511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -10504,7 +10534,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -10527,7 +10557,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -10547,7 +10577,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -10555,7 +10585,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -10563,7 +10593,7 @@
         <v>12264</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -10580,7 +10610,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -10615,7 +10645,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" style="2" bestFit="1" customWidth="1"/>
@@ -10623,7 +10653,7 @@
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -10634,7 +10664,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -10646,7 +10676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -10658,7 +10688,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -10670,7 +10700,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -10682,7 +10712,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -10694,7 +10724,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -10706,7 +10736,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -10728,17 +10758,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="14" width="20.75" style="16" customWidth="1"/>
     <col min="15" max="15" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A2," - ",'Troublepart of SP'!$C2)</f>
         <v>Report 2_6 - EXT_HISTORY_MASTER</v>
@@ -10775,7 +10805,7 @@
       </c>
       <c r="N1" s="26"/>
     </row>
-    <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1">
+    <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
@@ -10819,31 +10849,51 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:14" customFormat="1" ht="15" thickBot="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+    <row r="3" spans="1:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>17449200</v>
+      </c>
+      <c r="B3" s="19">
+        <v>403186</v>
+      </c>
+      <c r="C3" s="18">
+        <v>69409</v>
+      </c>
+      <c r="D3" s="19">
+        <v>83584</v>
+      </c>
+      <c r="E3" s="18">
+        <v>4557053</v>
+      </c>
+      <c r="F3" s="19">
+        <v>104503</v>
+      </c>
+      <c r="G3" s="18">
+        <v>17449200</v>
+      </c>
+      <c r="H3" s="19">
+        <v>1427</v>
+      </c>
+      <c r="I3" s="18">
+        <v>17449200</v>
+      </c>
+      <c r="J3" s="19">
+        <v>3413</v>
+      </c>
       <c r="K3" s="18">
-        <v>79738</v>
+        <v>69409</v>
       </c>
       <c r="L3" s="19">
-        <v>23580</v>
+        <v>18111</v>
       </c>
       <c r="M3" s="18">
-        <v>79738</v>
+        <v>69409</v>
       </c>
       <c r="N3" s="20">
-        <v>20500</v>
+        <v>15218</v>
       </c>
     </row>
-    <row r="4" spans="1:14" customFormat="1">
+    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10447188</v>
       </c>
@@ -10887,7 +10937,7 @@
         <v>10343</v>
       </c>
     </row>
-    <row r="5" spans="1:14" customFormat="1">
+    <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9706149</v>
       </c>
@@ -10931,7 +10981,7 @@
         <v>9671</v>
       </c>
     </row>
-    <row r="6" spans="1:14" customFormat="1">
+    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6945334</v>
       </c>
@@ -10975,7 +11025,7 @@
         <v>8947</v>
       </c>
     </row>
-    <row r="7" spans="1:14" customFormat="1">
+    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3726035</v>
       </c>
@@ -11019,7 +11069,7 @@
         <v>5278</v>
       </c>
     </row>
-    <row r="8" spans="1:14" customFormat="1">
+    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>280859</v>
       </c>
@@ -11063,7 +11113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" customFormat="1">
+    <row r="9" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
       <c r="D9" s="15"/>
       <c r="F9" s="15"/>
@@ -11071,7 +11121,7 @@
       <c r="J9" s="15"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:14" customFormat="1">
+    <row r="10" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
       <c r="D10" s="15"/>
       <c r="F10" s="15"/>
@@ -11079,7 +11129,7 @@
       <c r="J10" s="15"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:14" customFormat="1">
+    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
       <c r="D11" s="15"/>
       <c r="F11" s="15"/>
@@ -11087,7 +11137,7 @@
       <c r="J11" s="15"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:14" customFormat="1">
+    <row r="12" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
       <c r="D12" s="15"/>
       <c r="F12" s="15"/>
@@ -11095,7 +11145,7 @@
       <c r="J12" s="15"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:14" customFormat="1">
+    <row r="13" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
       <c r="D13" s="15"/>
       <c r="F13" s="15"/>
@@ -11103,7 +11153,7 @@
       <c r="J13" s="15"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:14" customFormat="1">
+    <row r="14" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
       <c r="D14" s="15"/>
       <c r="F14" s="15"/>
@@ -11111,7 +11161,7 @@
       <c r="J14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:14" customFormat="1">
+    <row r="15" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="D15" s="15"/>
       <c r="F15" s="15"/>
@@ -11119,7 +11169,7 @@
       <c r="J15" s="15"/>
       <c r="L15" s="15"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16" s="15"/>
       <c r="C16"/>
@@ -11155,17 +11205,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="14" width="20.75" style="16" customWidth="1"/>
     <col min="15" max="15" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A2," - ",'Troublepart of SP'!$C2)</f>
         <v>Report 2_6 - EXT_HISTORY_MASTER</v>
@@ -11202,7 +11252,7 @@
       </c>
       <c r="N1" s="26"/>
     </row>
-    <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1">
+    <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
@@ -11246,7 +11296,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:14" customFormat="1">
+    <row r="3" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10447188</v>
       </c>
@@ -11278,7 +11328,7 @@
       </c>
       <c r="N3" s="17"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1">
+    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>9706149</v>
       </c>
@@ -11309,7 +11359,7 @@
         <v>29876</v>
       </c>
     </row>
-    <row r="5" spans="1:14" customFormat="1">
+    <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6945334</v>
       </c>
@@ -11340,7 +11390,7 @@
         <v>19883</v>
       </c>
     </row>
-    <row r="6" spans="1:14" customFormat="1">
+    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3726035</v>
       </c>
@@ -11371,7 +11421,7 @@
         <v>11053</v>
       </c>
     </row>
-    <row r="7" spans="1:14" customFormat="1">
+    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>280859</v>
       </c>
@@ -11402,7 +11452,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="8" spans="1:14" customFormat="1">
+    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
       <c r="D8" s="15"/>
       <c r="F8" s="15"/>
@@ -11410,7 +11460,7 @@
       <c r="J8" s="15"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:14" customFormat="1">
+    <row r="9" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
       <c r="D9" s="15"/>
       <c r="F9" s="15"/>
@@ -11418,7 +11468,7 @@
       <c r="J9" s="15"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:14" customFormat="1">
+    <row r="10" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
       <c r="D10" s="15"/>
       <c r="F10" s="15"/>
@@ -11426,7 +11476,7 @@
       <c r="J10" s="15"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:14" customFormat="1">
+    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
       <c r="D11" s="15"/>
       <c r="F11" s="15"/>
@@ -11434,7 +11484,7 @@
       <c r="J11" s="15"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:14" customFormat="1">
+    <row r="12" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
       <c r="D12" s="15"/>
       <c r="F12" s="15"/>
@@ -11442,7 +11492,7 @@
       <c r="J12" s="15"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:14" customFormat="1">
+    <row r="13" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
       <c r="D13" s="15"/>
       <c r="F13" s="15"/>
@@ -11450,7 +11500,7 @@
       <c r="J13" s="15"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:14" customFormat="1">
+    <row r="14" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
       <c r="D14" s="15"/>
       <c r="F14" s="15"/>
@@ -11458,7 +11508,7 @@
       <c r="J14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:14" customFormat="1">
+    <row r="15" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="D15" s="15"/>
       <c r="F15" s="15"/>

</xml_diff>

<commit_message>
done with dropping parts of table
</commit_message>
<xml_diff>
--- a/Master Thesis/Analys/Experiments.xlsx
+++ b/Master Thesis/Analys/Experiments.xlsx
@@ -725,11 +725,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1086307728"/>
-        <c:axId val="-1086293584"/>
+        <c:axId val="1244420176"/>
+        <c:axId val="1244415824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1086307728"/>
+        <c:axId val="1244420176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +772,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086293584"/>
+        <c:crossAx val="1244415824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -780,7 +780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1086293584"/>
+        <c:axId val="1244415824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +831,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086307728"/>
+        <c:crossAx val="1244420176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1038,11 +1038,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1081216080"/>
-        <c:axId val="-1081210640"/>
+        <c:axId val="1249059568"/>
+        <c:axId val="1249050320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1081216080"/>
+        <c:axId val="1249059568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,12 +1099,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081210640"/>
+        <c:crossAx val="1249050320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1081210640"/>
+        <c:axId val="1249050320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,7 +1161,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081216080"/>
+        <c:crossAx val="1249059568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1303,11 +1303,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1081205200"/>
-        <c:axId val="-1081213904"/>
+        <c:axId val="1249053584"/>
+        <c:axId val="1249059024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1081205200"/>
+        <c:axId val="1249053584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1364,12 +1364,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081213904"/>
+        <c:crossAx val="1249059024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1081213904"/>
+        <c:axId val="1249059024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,7 +1426,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081205200"/>
+        <c:crossAx val="1249053584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1568,11 +1568,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1081211728"/>
-        <c:axId val="-1081211184"/>
+        <c:axId val="1249047600"/>
+        <c:axId val="1249048144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1081211728"/>
+        <c:axId val="1249047600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,12 +1629,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081211184"/>
+        <c:crossAx val="1249048144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1081211184"/>
+        <c:axId val="1249048144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,7 +1691,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081211728"/>
+        <c:crossAx val="1249047600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1833,11 +1833,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1043475920"/>
-        <c:axId val="-1043477008"/>
+        <c:axId val="1248831840"/>
+        <c:axId val="1248843264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1043475920"/>
+        <c:axId val="1248831840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1894,12 +1894,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1043477008"/>
+        <c:crossAx val="1248843264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1043477008"/>
+        <c:axId val="1248843264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,7 +1956,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1043475920"/>
+        <c:crossAx val="1248831840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2098,11 +2098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1043480272"/>
-        <c:axId val="-1043484624"/>
+        <c:axId val="1248841088"/>
+        <c:axId val="1248834016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1043480272"/>
+        <c:axId val="1248841088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2159,12 +2159,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1043484624"/>
+        <c:crossAx val="1248834016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1043484624"/>
+        <c:axId val="1248834016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +2221,537 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1043480272"/>
+        <c:crossAx val="1248841088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Table content drop w I&amp;Keys'!$K$3:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>39869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29876</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19883</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11053</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>724</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Table content drop w I&amp;Keys'!$L$3:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12072</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10257</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1279446352"/>
+        <c:axId val="1279439824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1279446352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279439824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1279439824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279446352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Table content drop w I&amp;Keys'!$M$3:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>39869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29876</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19883</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11053</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>724</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Table content drop w I&amp;Keys'!$N$3:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10093</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9119</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8647</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4949</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1279440368"/>
+        <c:axId val="1279443632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1279440368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279443632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1279443632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279440368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2285,7 +2815,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2791,11 +3320,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1086294672"/>
-        <c:axId val="-1086294128"/>
+        <c:axId val="1244413104"/>
+        <c:axId val="1244404944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1086294672"/>
+        <c:axId val="1244413104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2838,7 +3367,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086294128"/>
+        <c:crossAx val="1244404944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2846,7 +3375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1086294128"/>
+        <c:axId val="1244404944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2897,7 +3426,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086294672"/>
+        <c:crossAx val="1244413104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2911,7 +3440,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3077,11 +3605,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1086301744"/>
-        <c:axId val="-1086308272"/>
+        <c:axId val="1244418000"/>
+        <c:axId val="1244411472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1086301744"/>
+        <c:axId val="1244418000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3138,12 +3666,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086308272"/>
+        <c:crossAx val="1244411472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1086308272"/>
+        <c:axId val="1244411472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3200,7 +3728,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086301744"/>
+        <c:crossAx val="1244418000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3348,11 +3876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1086301200"/>
-        <c:axId val="-1086304464"/>
+        <c:axId val="1244406032"/>
+        <c:axId val="1244406576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1086301200"/>
+        <c:axId val="1244406032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3409,12 +3937,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086304464"/>
+        <c:crossAx val="1244406576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1086304464"/>
+        <c:axId val="1244406576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3471,7 +3999,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086301200"/>
+        <c:crossAx val="1244406032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3619,11 +4147,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1086303920"/>
-        <c:axId val="-1086303376"/>
+        <c:axId val="1244409840"/>
+        <c:axId val="1244410384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1086303920"/>
+        <c:axId val="1244409840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3680,12 +4208,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086303376"/>
+        <c:crossAx val="1244410384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1086303376"/>
+        <c:axId val="1244410384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3742,7 +4270,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1086303920"/>
+        <c:crossAx val="1244409840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3890,11 +4418,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1081205744"/>
-        <c:axId val="-1081203568"/>
+        <c:axId val="1249054128"/>
+        <c:axId val="1249053040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1081205744"/>
+        <c:axId val="1249054128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3951,12 +4479,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081203568"/>
+        <c:crossAx val="1249053040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1081203568"/>
+        <c:axId val="1249053040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4013,7 +4541,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081205744"/>
+        <c:crossAx val="1249054128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4161,11 +4689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1081217712"/>
-        <c:axId val="-1081213360"/>
+        <c:axId val="1249061200"/>
+        <c:axId val="1249051408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1081217712"/>
+        <c:axId val="1249061200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4222,12 +4750,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081213360"/>
+        <c:crossAx val="1249051408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1081213360"/>
+        <c:axId val="1249051408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4284,7 +4812,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081217712"/>
+        <c:crossAx val="1249061200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4432,11 +4960,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1081204656"/>
-        <c:axId val="-1081208464"/>
+        <c:axId val="1249055760"/>
+        <c:axId val="1249049232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1081204656"/>
+        <c:axId val="1249055760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4493,12 +5021,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081208464"/>
+        <c:crossAx val="1249049232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1081208464"/>
+        <c:axId val="1249049232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4555,7 +5083,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081204656"/>
+        <c:crossAx val="1249055760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4703,11 +5231,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1081207920"/>
-        <c:axId val="-1081206832"/>
+        <c:axId val="1249061744"/>
+        <c:axId val="1249051952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1081207920"/>
+        <c:axId val="1249061744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4764,12 +5292,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081206832"/>
+        <c:crossAx val="1249051952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1081206832"/>
+        <c:axId val="1249051952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4826,7 +5354,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1081207920"/>
+        <c:crossAx val="1249061744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5076,6 +5604,86 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8003,6 +8611,1038 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13078,6 +14718,70 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14684,8 +16388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14809,11 +16513,15 @@
       <c r="K3" s="10">
         <v>39869</v>
       </c>
-      <c r="L3" s="15"/>
+      <c r="L3" s="15">
+        <v>12072</v>
+      </c>
       <c r="M3" s="10">
         <v>39869</v>
       </c>
-      <c r="N3" s="17"/>
+      <c r="N3" s="17">
+        <v>10093</v>
+      </c>
     </row>
     <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -14849,9 +16557,14 @@
       <c r="K4" s="10">
         <v>29876</v>
       </c>
-      <c r="L4" s="15"/>
+      <c r="L4" s="15">
+        <v>11029</v>
+      </c>
       <c r="M4" s="10">
         <v>29876</v>
+      </c>
+      <c r="N4">
+        <v>9119</v>
       </c>
     </row>
     <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
@@ -14888,9 +16601,14 @@
       <c r="K5" s="10">
         <v>19883</v>
       </c>
-      <c r="L5" s="15"/>
+      <c r="L5" s="15">
+        <v>10257</v>
+      </c>
       <c r="M5" s="10">
         <v>19883</v>
+      </c>
+      <c r="N5">
+        <v>8647</v>
       </c>
     </row>
     <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
@@ -14927,9 +16645,14 @@
       <c r="K6" s="10">
         <v>11053</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="15">
+        <v>5996</v>
+      </c>
       <c r="M6" s="10">
         <v>11053</v>
+      </c>
+      <c r="N6">
+        <v>4949</v>
       </c>
     </row>
     <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
@@ -14966,9 +16689,14 @@
       <c r="K7" s="10">
         <v>724</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="15">
+        <v>58</v>
+      </c>
       <c r="M7" s="10">
         <v>724</v>
+      </c>
+      <c r="N7">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed index alterations images
</commit_message>
<xml_diff>
--- a/Master Thesis/Analys/Experiments.xlsx
+++ b/Master Thesis/Analys/Experiments.xlsx
@@ -245,7 +245,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -783,11 +783,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1902001888"/>
-        <c:axId val="1902002432"/>
+        <c:axId val="1214925584"/>
+        <c:axId val="1214927216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1902001888"/>
+        <c:axId val="1214925584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +830,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1902002432"/>
+        <c:crossAx val="1214927216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,7 +838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1902002432"/>
+        <c:axId val="1214927216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +889,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1902001888"/>
+        <c:crossAx val="1214925584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1151,11 +1151,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2084285536"/>
-        <c:axId val="2084290976"/>
+        <c:axId val="1217965424"/>
+        <c:axId val="1218152896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2084285536"/>
+        <c:axId val="1217965424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,12 +1270,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084290976"/>
+        <c:crossAx val="1218152896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084290976"/>
+        <c:axId val="1218152896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1387,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084285536"/>
+        <c:crossAx val="1217965424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1584,11 +1584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2084287712"/>
-        <c:axId val="2084289344"/>
+        <c:axId val="1218154528"/>
+        <c:axId val="1218153984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2084287712"/>
+        <c:axId val="1218154528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,12 +1703,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084289344"/>
+        <c:crossAx val="1218153984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084289344"/>
+        <c:axId val="1218153984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1820,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084287712"/>
+        <c:crossAx val="1218154528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2017,11 +2017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2084289888"/>
-        <c:axId val="2084290432"/>
+        <c:axId val="1218148544"/>
+        <c:axId val="1218149088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2084289888"/>
+        <c:axId val="1218148544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,12 +2136,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084290432"/>
+        <c:crossAx val="1218149088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084290432"/>
+        <c:axId val="1218149088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,7 +2253,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084289888"/>
+        <c:crossAx val="1218148544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2450,11 +2450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083663024"/>
-        <c:axId val="2083659760"/>
+        <c:axId val="1218153440"/>
+        <c:axId val="1218151808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083663024"/>
+        <c:axId val="1218153440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2569,12 +2569,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083659760"/>
+        <c:crossAx val="1218151808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083659760"/>
+        <c:axId val="1218151808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2686,7 +2686,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083663024"/>
+        <c:crossAx val="1218153440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2883,11 +2883,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083660848"/>
-        <c:axId val="2083666288"/>
+        <c:axId val="1219627216"/>
+        <c:axId val="1219622320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083660848"/>
+        <c:axId val="1219627216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3002,12 +3002,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083666288"/>
+        <c:crossAx val="1219622320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083666288"/>
+        <c:axId val="1219622320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3119,7 +3119,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083660848"/>
+        <c:crossAx val="1219627216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3316,11 +3316,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083661392"/>
-        <c:axId val="2083664112"/>
+        <c:axId val="1219625040"/>
+        <c:axId val="1219627760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083661392"/>
+        <c:axId val="1219625040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,12 +3435,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083664112"/>
+        <c:crossAx val="1219627760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083664112"/>
+        <c:axId val="1219627760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3552,7 +3552,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083661392"/>
+        <c:crossAx val="1219625040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3749,11 +3749,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083661936"/>
-        <c:axId val="2085025872"/>
+        <c:axId val="1219625584"/>
+        <c:axId val="1219629392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083661936"/>
+        <c:axId val="1219625584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3868,12 +3868,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085025872"/>
+        <c:crossAx val="1219629392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2085025872"/>
+        <c:axId val="1219629392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3985,7 +3985,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083661936"/>
+        <c:crossAx val="1219625584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4127,11 +4127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085023152"/>
-        <c:axId val="2085034576"/>
+        <c:axId val="1219628848"/>
+        <c:axId val="1219497744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085023152"/>
+        <c:axId val="1219628848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4188,12 +4188,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085034576"/>
+        <c:crossAx val="1219497744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2085034576"/>
+        <c:axId val="1219497744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4250,7 +4250,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085023152"/>
+        <c:crossAx val="1219628848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4392,11 +4392,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085026416"/>
-        <c:axId val="2085031856"/>
+        <c:axId val="1219504816"/>
+        <c:axId val="1219502096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085026416"/>
+        <c:axId val="1219504816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4453,12 +4453,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085031856"/>
+        <c:crossAx val="1219502096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2085031856"/>
+        <c:axId val="1219502096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4515,7 +4515,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085026416"/>
+        <c:crossAx val="1219504816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4712,11 +4712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085026960"/>
-        <c:axId val="2085028592"/>
+        <c:axId val="1219499920"/>
+        <c:axId val="1219503184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085026960"/>
+        <c:axId val="1219499920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4828,12 +4828,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085028592"/>
+        <c:crossAx val="1219503184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2085028592"/>
+        <c:axId val="1219503184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4945,7 +4945,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085026960"/>
+        <c:crossAx val="1219499920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5484,11 +5484,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2083351936"/>
-        <c:axId val="2083363904"/>
+        <c:axId val="1214922864"/>
+        <c:axId val="1214923408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2083351936"/>
+        <c:axId val="1214922864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5531,7 +5531,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083363904"/>
+        <c:crossAx val="1214923408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5539,7 +5539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083363904"/>
+        <c:axId val="1214923408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5645,7 +5645,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083351936"/>
+        <c:crossAx val="1214922864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5802,24 +5802,23 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Playing with indexes HISTOR '!$A$2:$A$11</c:f>
@@ -5897,7 +5896,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5907,17 +5905,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2085023696"/>
-        <c:axId val="2085024240"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="1219502640"/>
+        <c:axId val="1219501008"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2085023696"/>
+        <c:axId val="1219502640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5955,7 +5953,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085024240"/>
+        <c:crossAx val="1219501008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5963,12 +5961,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085024240"/>
+        <c:axId val="1219501008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -5986,7 +5984,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -6019,7 +6017,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -6070,7 +6068,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085023696"/>
+        <c:crossAx val="1219502640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6196,24 +6194,23 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Playing with indexes HISTOR '!$A$2:$A$11</c:f>
@@ -6291,7 +6288,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6301,17 +6297,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2085036208"/>
-        <c:axId val="2085020976"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="1219909744"/>
+        <c:axId val="1219913008"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2085036208"/>
+        <c:axId val="1219909744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6349,7 +6345,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085020976"/>
+        <c:crossAx val="1219913008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6357,12 +6353,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085020976"/>
+        <c:axId val="1219913008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -6380,7 +6376,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -6413,7 +6409,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -6464,7 +6460,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085036208"/>
+        <c:crossAx val="1219909744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6590,24 +6586,23 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Playing with indexes HISTOR '!$A$2:$A$11</c:f>
@@ -6685,7 +6680,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6695,17 +6689,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2085032400"/>
-        <c:axId val="2085024784"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="1219915184"/>
+        <c:axId val="1219915728"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2085032400"/>
+        <c:axId val="1219915184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6743,7 +6737,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085024784"/>
+        <c:crossAx val="1219915728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6751,12 +6745,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085024784"/>
+        <c:axId val="1219915728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -6774,7 +6768,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -6807,7 +6801,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -6858,7 +6852,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085032400"/>
+        <c:crossAx val="1219915184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7061,11 +7055,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083350848"/>
-        <c:axId val="2083365536"/>
+        <c:axId val="1214924496"/>
+        <c:axId val="1214917424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083350848"/>
+        <c:axId val="1214924496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7177,12 +7171,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083365536"/>
+        <c:crossAx val="1214917424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083365536"/>
+        <c:axId val="1214917424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7294,7 +7288,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083350848"/>
+        <c:crossAx val="1214924496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7497,11 +7491,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083353568"/>
-        <c:axId val="2083357920"/>
+        <c:axId val="1214922320"/>
+        <c:axId val="1214931024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083353568"/>
+        <c:axId val="1214922320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7616,12 +7610,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083357920"/>
+        <c:crossAx val="1214931024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083357920"/>
+        <c:axId val="1214931024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7733,7 +7727,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083353568"/>
+        <c:crossAx val="1214922320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7936,11 +7930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083360640"/>
-        <c:axId val="2083356288"/>
+        <c:axId val="1214928304"/>
+        <c:axId val="1214919056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083360640"/>
+        <c:axId val="1214928304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8055,12 +8049,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083356288"/>
+        <c:crossAx val="1214919056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083356288"/>
+        <c:axId val="1214919056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8172,7 +8166,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083360640"/>
+        <c:crossAx val="1214928304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8375,11 +8369,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083359552"/>
-        <c:axId val="2083351392"/>
+        <c:axId val="1214929936"/>
+        <c:axId val="1214928848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083359552"/>
+        <c:axId val="1214929936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8494,12 +8488,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083351392"/>
+        <c:crossAx val="1214928848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083351392"/>
+        <c:axId val="1214928848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8611,7 +8605,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083359552"/>
+        <c:crossAx val="1214929936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8814,11 +8808,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083354112"/>
-        <c:axId val="2083362272"/>
+        <c:axId val="1217963792"/>
+        <c:axId val="1217965968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083354112"/>
+        <c:axId val="1217963792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8933,12 +8927,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083362272"/>
+        <c:crossAx val="1217965968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083362272"/>
+        <c:axId val="1217965968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9050,7 +9044,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083354112"/>
+        <c:crossAx val="1217963792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9253,11 +9247,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083362816"/>
-        <c:axId val="2083364448"/>
+        <c:axId val="1217968144"/>
+        <c:axId val="1217967056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083362816"/>
+        <c:axId val="1217968144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9372,12 +9366,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083364448"/>
+        <c:crossAx val="1217967056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083364448"/>
+        <c:axId val="1217967056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9489,7 +9483,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083362816"/>
+        <c:crossAx val="1217968144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9692,11 +9686,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083350304"/>
-        <c:axId val="2084287168"/>
+        <c:axId val="1217964336"/>
+        <c:axId val="1217964880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083350304"/>
+        <c:axId val="1217964336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9811,12 +9805,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2084287168"/>
+        <c:crossAx val="1217964880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2084287168"/>
+        <c:axId val="1217964880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9928,7 +9922,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083350304"/>
+        <c:crossAx val="1217964336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23185,9 +23179,9 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -23195,7 +23189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -23203,7 +23197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -23211,7 +23205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -23219,7 +23213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -23227,7 +23221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -23235,7 +23229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -23243,7 +23237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -23264,15 +23258,15 @@
       <selection activeCell="B11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="21" t="s">
         <v>8</v>
@@ -23280,7 +23274,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -23294,7 +23288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickTop="1">
+    <row r="3" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -23309,7 +23303,7 @@
         <v>427017</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -23324,7 +23318,7 @@
         <v>202116</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -23339,7 +23333,7 @@
         <v>147443</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -23354,7 +23348,7 @@
         <v>33168</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -23369,7 +23363,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -23384,7 +23378,7 @@
         <v>21785</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -23399,7 +23393,7 @@
         <v>10634</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -23414,7 +23408,7 @@
         <v>9522</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -23429,7 +23423,7 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -23444,7 +23438,7 @@
         <v>12655</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -23459,7 +23453,7 @@
         <v>8998</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -23474,7 +23468,7 @@
         <v>11381</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -23489,7 +23483,7 @@
         <v>6429</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -23504,7 +23498,7 @@
         <v>6347</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -23519,7 +23513,7 @@
         <v>6249</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
@@ -23534,7 +23528,7 @@
         <v>5973</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -23549,7 +23543,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -23564,7 +23558,7 @@
         <v>3433</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
@@ -23579,7 +23573,7 @@
         <v>5483</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>32</v>
       </c>
@@ -23594,7 +23588,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
@@ -23609,7 +23603,7 @@
         <v>3960</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
@@ -23624,7 +23618,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -23639,7 +23633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -23654,7 +23648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>37</v>
       </c>
@@ -23669,7 +23663,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -23684,7 +23678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
@@ -23699,7 +23693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -23714,7 +23708,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
@@ -23729,7 +23723,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>42</v>
       </c>
@@ -23744,7 +23738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" ht="15" thickTop="1"/>
+    <row r="33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
@@ -23762,13 +23756,13 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="23" t="s">
         <v>45</v>
       </c>
@@ -23778,7 +23772,7 @@
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -23801,7 +23795,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -23824,7 +23818,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -23847,7 +23841,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -23867,7 +23861,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -23875,7 +23869,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -23883,7 +23877,7 @@
         <v>12264</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -23900,7 +23894,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -23935,15 +23929,15 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -23954,7 +23948,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -23966,7 +23960,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -23978,7 +23972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -23990,7 +23984,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -24002,7 +23996,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -24014,7 +24008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -24026,7 +24020,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -24052,13 +24046,13 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="20.75" style="16" customWidth="1"/>
+    <col min="1" max="14" width="20.7109375" style="16" customWidth="1"/>
     <col min="15" max="15" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A2," - ",'Troublepart of SP'!$C2)</f>
         <v>Report 2_6 - EXT_HISTORY_MASTER</v>
@@ -24095,7 +24089,7 @@
       </c>
       <c r="N1" s="26"/>
     </row>
-    <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1">
+    <row r="2" spans="1:14" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
@@ -24139,7 +24133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:14" customFormat="1" ht="15" thickBot="1">
+    <row r="3" spans="1:14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>17449200</v>
       </c>
@@ -24183,7 +24177,7 @@
         <v>15218</v>
       </c>
     </row>
-    <row r="4" spans="1:14" customFormat="1">
+    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10447188</v>
       </c>
@@ -24227,7 +24221,7 @@
         <v>10343</v>
       </c>
     </row>
-    <row r="5" spans="1:14" customFormat="1">
+    <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9706149</v>
       </c>
@@ -24271,7 +24265,7 @@
         <v>9671</v>
       </c>
     </row>
-    <row r="6" spans="1:14" customFormat="1">
+    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6945334</v>
       </c>
@@ -24315,7 +24309,7 @@
         <v>8947</v>
       </c>
     </row>
-    <row r="7" spans="1:14" customFormat="1">
+    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3726035</v>
       </c>
@@ -24359,7 +24353,7 @@
         <v>5278</v>
       </c>
     </row>
-    <row r="8" spans="1:14" customFormat="1">
+    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>280859</v>
       </c>
@@ -24403,7 +24397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" customFormat="1">
+    <row r="9" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="D9" s="15"/>
       <c r="F9" s="15"/>
@@ -24411,7 +24405,7 @@
       <c r="J9" s="15"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:14" customFormat="1">
+    <row r="10" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="D10" s="15"/>
       <c r="F10" s="15"/>
@@ -24419,7 +24413,7 @@
       <c r="J10" s="15"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:14" customFormat="1">
+    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="D11" s="15"/>
       <c r="F11" s="15"/>
@@ -24427,7 +24421,7 @@
       <c r="J11" s="15"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:14" customFormat="1">
+    <row r="12" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="D12" s="15"/>
       <c r="F12" s="15"/>
@@ -24435,7 +24429,7 @@
       <c r="J12" s="15"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:14" customFormat="1">
+    <row r="13" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="D13" s="15"/>
       <c r="F13" s="15"/>
@@ -24443,7 +24437,7 @@
       <c r="J13" s="15"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:14" customFormat="1">
+    <row r="14" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="D14" s="15"/>
       <c r="F14" s="15"/>
@@ -24451,7 +24445,7 @@
       <c r="J14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:14" customFormat="1">
+    <row r="15" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="D15" s="15"/>
       <c r="F15" s="15"/>
@@ -24459,7 +24453,7 @@
       <c r="J15" s="15"/>
       <c r="L15" s="15"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16" s="15"/>
       <c r="C16"/>
@@ -24499,13 +24493,13 @@
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="20.75" style="16" customWidth="1"/>
+    <col min="1" max="14" width="20.7109375" style="16" customWidth="1"/>
     <col min="15" max="15" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="str">
         <f>CONCATENATE('Troublepart of SP'!$A2," - ",'Troublepart of SP'!$C2)</f>
         <v>Report 2_6 - EXT_HISTORY_MASTER</v>
@@ -24542,7 +24536,7 @@
       </c>
       <c r="N1" s="26"/>
     </row>
-    <row r="2" spans="1:14" customFormat="1" ht="15.75" thickTop="1" thickBot="1">
+    <row r="2" spans="1:14" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
@@ -24586,7 +24580,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:14" customFormat="1">
+    <row r="3" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10447188</v>
       </c>
@@ -24630,7 +24624,7 @@
         <v>10093</v>
       </c>
     </row>
-    <row r="4" spans="1:14" customFormat="1">
+    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9706149</v>
       </c>
@@ -24674,7 +24668,7 @@
         <v>9119</v>
       </c>
     </row>
-    <row r="5" spans="1:14" customFormat="1">
+    <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6945334</v>
       </c>
@@ -24718,7 +24712,7 @@
         <v>8647</v>
       </c>
     </row>
-    <row r="6" spans="1:14" customFormat="1">
+    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3726035</v>
       </c>
@@ -24762,7 +24756,7 @@
         <v>4949</v>
       </c>
     </row>
-    <row r="7" spans="1:14" customFormat="1">
+    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>280859</v>
       </c>
@@ -24806,7 +24800,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:14" customFormat="1">
+    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="D8" s="15"/>
       <c r="F8" s="15"/>
@@ -24814,7 +24808,7 @@
       <c r="J8" s="15"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:14" customFormat="1">
+    <row r="9" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="D9" s="15"/>
       <c r="F9" s="15"/>
@@ -24822,7 +24816,7 @@
       <c r="J9" s="15"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:14" customFormat="1">
+    <row r="10" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="D10" s="15"/>
       <c r="F10" s="15"/>
@@ -24830,7 +24824,7 @@
       <c r="J10" s="15"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:14" customFormat="1">
+    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="D11" s="15"/>
       <c r="F11" s="15"/>
@@ -24838,7 +24832,7 @@
       <c r="J11" s="15"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:14" customFormat="1">
+    <row r="12" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="D12" s="15"/>
       <c r="F12" s="15"/>
@@ -24846,7 +24840,7 @@
       <c r="J12" s="15"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:14" customFormat="1">
+    <row r="13" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="D13" s="15"/>
       <c r="F13" s="15"/>
@@ -24854,7 +24848,7 @@
       <c r="J13" s="15"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:14" customFormat="1">
+    <row r="14" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="D14" s="15"/>
       <c r="F14" s="15"/>
@@ -24862,7 +24856,7 @@
       <c r="J14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:14" customFormat="1">
+    <row r="15" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="D15" s="15"/>
       <c r="F15" s="15"/>
@@ -24870,7 +24864,7 @@
       <c r="J15" s="15"/>
       <c r="L15" s="15"/>
     </row>
-    <row r="34" spans="3:14" ht="15" thickBot="1">
+    <row r="34" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="26" t="s">
         <v>54</v>
       </c>
@@ -24888,7 +24882,7 @@
       </c>
       <c r="N34" s="27"/>
     </row>
-    <row r="35" spans="3:14" ht="15.75" thickTop="1" thickBot="1">
+    <row r="35" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="11" t="s">
         <v>51</v>
       </c>
@@ -24914,7 +24908,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="3:14">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>10447188</v>
       </c>
@@ -24938,7 +24932,7 @@
         <v>10158</v>
       </c>
     </row>
-    <row r="37" spans="3:14">
+    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>9706149</v>
       </c>
@@ -24962,7 +24956,7 @@
         <v>10062</v>
       </c>
     </row>
-    <row r="38" spans="3:14">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>6945334</v>
       </c>
@@ -24986,7 +24980,7 @@
         <v>9943</v>
       </c>
     </row>
-    <row r="39" spans="3:14">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>3726035</v>
       </c>
@@ -25010,7 +25004,7 @@
         <v>9855</v>
       </c>
     </row>
-    <row r="40" spans="3:14">
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>280859</v>
       </c>
@@ -25034,56 +25028,56 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="3:14">
+    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C41"/>
       <c r="D41" s="15"/>
       <c r="F41" s="15"/>
       <c r="K41" s="17"/>
       <c r="L41" s="15"/>
     </row>
-    <row r="42" spans="3:14">
+    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C42"/>
       <c r="D42" s="15"/>
       <c r="F42" s="15"/>
       <c r="K42" s="17"/>
       <c r="L42" s="15"/>
     </row>
-    <row r="43" spans="3:14">
+    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C43"/>
       <c r="D43" s="15"/>
       <c r="F43" s="15"/>
       <c r="K43" s="17"/>
       <c r="L43" s="15"/>
     </row>
-    <row r="44" spans="3:14">
+    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C44"/>
       <c r="D44" s="15"/>
       <c r="F44" s="15"/>
       <c r="K44" s="17"/>
       <c r="L44" s="15"/>
     </row>
-    <row r="45" spans="3:14">
+    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C45"/>
       <c r="D45" s="15"/>
       <c r="F45" s="15"/>
       <c r="K45" s="17"/>
       <c r="L45" s="15"/>
     </row>
-    <row r="46" spans="3:14">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C46"/>
       <c r="D46" s="15"/>
       <c r="F46" s="15"/>
       <c r="K46" s="17"/>
       <c r="L46" s="15"/>
     </row>
-    <row r="47" spans="3:14">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C47"/>
       <c r="D47" s="15"/>
       <c r="F47" s="15"/>
       <c r="K47" s="17"/>
       <c r="L47" s="15"/>
     </row>
-    <row r="48" spans="3:14">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C48"/>
       <c r="D48" s="15"/>
       <c r="F48" s="15"/>
@@ -25092,17 +25086,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="K34:L34"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25114,19 +25108,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>61</v>
       </c>
@@ -25140,7 +25134,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -25154,7 +25148,7 @@
         <v>18111</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -25168,7 +25162,7 @@
         <v>12512</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -25182,7 +25176,7 @@
         <v>6763</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -25199,7 +25193,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -25216,7 +25210,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -25233,7 +25227,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -25250,7 +25244,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -25267,7 +25261,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -25284,7 +25278,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>

</xml_diff>